<commit_message>
Deploying to gh-pages from @ eurovibes/LEDcube@a7234f0d9a771873ee846fc7fcf68f8b4e66b4fe 🚀
</commit_message>
<xml_diff>
--- a/Fabrication/BoM/LEDcube-bom_v0.1.xlsx
+++ b/Fabrication/BoM/LEDcube-bom_v0.1.xlsx
@@ -170,7 +170,7 @@
     <t>9</t>
   </si>
   <si>
-    <t>R101 R102</t>
+    <t>R101 R102 R103</t>
   </si>
   <si>
     <t>R</t>
@@ -263,7 +263,7 @@
     <t>KiCad Version:</t>
   </si>
   <si>
-    <t>6.0.4+dfsg-1~bpo11+1</t>
+    <t>6.0.5+dfsg-1~bpo11+1</t>
   </si>
   <si>
     <t>Component Groups:</t>
@@ -815,7 +815,7 @@
         <v>83</v>
       </c>
       <c r="F3" s="3">
-        <v>26</v>
+        <v>27</v>
       </c>
     </row>
     <row r="4" spans="1:10">
@@ -829,7 +829,7 @@
         <v>84</v>
       </c>
       <c r="F4" s="3">
-        <v>26</v>
+        <v>27</v>
       </c>
     </row>
     <row r="5" spans="1:10">
@@ -857,7 +857,7 @@
         <v>86</v>
       </c>
       <c r="F6" s="3">
-        <v>26</v>
+        <v>27</v>
       </c>
     </row>
     <row r="8" spans="1:10">
@@ -1177,7 +1177,7 @@
         <v>14</v>
       </c>
       <c r="J17" s="5" t="s">
-        <v>17</v>
+        <v>22</v>
       </c>
     </row>
     <row r="18" spans="1:10">

</xml_diff>